<commit_message>
FIX: quit error in GazeParserrCheck and GazeParserInit
</commit_message>
<xml_diff>
--- a/Samples/component_sample02/sample02.xlsx
+++ b/Samples/component_sample02/sample02.xlsx
@@ -381,7 +381,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -399,7 +399,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2">
-        <v>1.3</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="B2">
         <v>-400</v>
@@ -410,7 +410,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3">
-        <v>1.3</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="B3">
         <v>-400</v>
@@ -421,7 +421,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>1.3</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="B4">
         <v>-400</v>
@@ -432,7 +432,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5">
-        <v>1.3</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="B5">
         <v>-400</v>
@@ -443,7 +443,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>1.3</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="B6">
         <v>-400</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>1.3</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="B7">
         <v>400</v>
@@ -465,7 +465,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>1.3</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="B8">
         <v>400</v>
@@ -476,7 +476,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>1.3</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="B9">
         <v>400</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>1.3</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="B10">
         <v>400</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>1.3</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="B11">
         <v>400</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="B12">
         <v>-400</v>
@@ -520,7 +520,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="B13">
         <v>-400</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="B14">
         <v>-400</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="B15">
         <v>-400</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="B16">
         <v>-400</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="B17">
         <v>400</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="B18">
         <v>400</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="B19">
         <v>400</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="B20">
         <v>400</v>
@@ -608,7 +608,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="B21">
         <v>400</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B22">
         <v>-400</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B23">
         <v>-400</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B24">
         <v>-400</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B25">
         <v>-400</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B26">
         <v>-400</v>
@@ -674,7 +674,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B27">
         <v>400</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B28">
         <v>400</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B29">
         <v>400</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B30">
         <v>400</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>1.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B31">
         <v>400</v>

</xml_diff>

<commit_message>
MOD: change parameters in component_sample02
</commit_message>
<xml_diff>
--- a/Samples/component_sample02/sample02.xlsx
+++ b/Samples/component_sample02/sample02.xlsx
@@ -381,7 +381,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -399,7 +399,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2">
-        <v>1.7999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="B2">
         <v>-400</v>
@@ -410,7 +410,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3">
-        <v>1.7999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="B3">
         <v>-400</v>
@@ -421,7 +421,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>1.7999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="B4">
         <v>-400</v>
@@ -432,7 +432,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5">
-        <v>1.7999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="B5">
         <v>-400</v>
@@ -443,7 +443,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>1.7999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="B6">
         <v>-400</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>1.7999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="B7">
         <v>400</v>
@@ -465,7 +465,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>1.7999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="B8">
         <v>400</v>
@@ -476,7 +476,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>1.7999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="B9">
         <v>400</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>1.7999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="B10">
         <v>400</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>1.7999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="B11">
         <v>400</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B12">
         <v>-400</v>
@@ -520,7 +520,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B13">
         <v>-400</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B14">
         <v>-400</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B15">
         <v>-400</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B16">
         <v>-400</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B17">
         <v>400</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B18">
         <v>400</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B19">
         <v>400</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B20">
         <v>400</v>
@@ -608,7 +608,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B21">
         <v>400</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="B22">
         <v>-400</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="B23">
         <v>-400</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="B24">
         <v>-400</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="B25">
         <v>-400</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="B26">
         <v>-400</v>
@@ -674,7 +674,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="B27">
         <v>400</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="B28">
         <v>400</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="B29">
         <v>400</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="B30">
         <v>400</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>2.2000000000000002</v>
+        <v>1.7</v>
       </c>
       <c r="B31">
         <v>400</v>

</xml_diff>